<commit_message>
handle excel to json
</commit_message>
<xml_diff>
--- a/datas/excel_datas/陶瓷.xlsx
+++ b/datas/excel_datas/陶瓷.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S10"/>
+  <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -526,7 +526,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://www.xiaohongshu.com/explore/663b40c9000000001e023f05?xsec_token=AB4IeNurF0eRCB8znUVFqHPtzD4mxrB0pbKxdjzAY9-_o=</t>
+          <t>https://www.xiaohongshu.com/explore/663b40c9000000001e023f05?xsec_token=AB4IeNurF0eRCB8znUVFqHPhOH6jpm3irRSF-Dp_e718w=</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -576,7 +576,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>2242</t>
+          <t>2243</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
@@ -596,7 +596,7 @@
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>['http://sns-webpic-qc.xhscdn.com/202504302109/7f3b70d62f7da6a35843b0fd39e9d9f2/1040g008312hhssb6na505p6s7ec08k6pk8bdjr0!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202504302109/0d1063f9c59ef9d54e92db78550edfaf/1040g008312hhssb6na6g5p6s7ec08k6p0j1abj0!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202504302109/df62f770afd18039027e67361166df7a/1040g008312hhssb6na4g5p6s7ec08k6p33s9d5g!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202504302109/b9232abbfb10f3949a1341ab692a4ca7/1040g008312hhssb6na405p6s7ec08k6pjoj6s48!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202504302109/3823c1915fbbf5de8861e95f9f8d71bb/1040g008312hhssb6na2g5p6s7ec08k6pf5eat08!nd_dft_wlteh_webp_3']</t>
+          <t>['http://sns-webpic-qc.xhscdn.com/202505012057/caf27ac7804eca609704fcc2237aa5d3/1040g008312hhssb6na505p6s7ec08k6pk8bdjr0!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202505012057/81836421a5f32988fbc670a399bb8045/1040g008312hhssb6na6g5p6s7ec08k6p0j1abj0!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202505012057/7e924ee01f27dc0921df45bfcb875a01/1040g008312hhssb6na4g5p6s7ec08k6p33s9d5g!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202505012057/98666eb581037f58c19d8d13c4b648ec/1040g008312hhssb6na405p6s7ec08k6pjoj6s48!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202505012057/e1b81076a5ba1037aeb1fc502a268b65/1040g008312hhssb6na2g5p6s7ec08k6pf5eat08!nd_dft_wlteh_webp_3']</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
@@ -623,7 +623,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://www.xiaohongshu.com/explore/6763a5d7000000000b00f14c?xsec_token=ABFbNNQ_Tw0xWq2ZAOWfZ5ZFvnB8A7Xhz-rrftfZRnZyk=</t>
+          <t>https://www.xiaohongshu.com/explore/6763a5d7000000000b00f14c?xsec_token=ABFbNNQ_Tw0xWq2ZAOWfZ5ZHVGk1Go_orOF-7d8f1luDk=</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -671,22 +671,22 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>381</t>
+          <t>390</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>157</t>
+          <t>158</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>58</t>
+          <t>59</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
@@ -701,7 +701,7 @@
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>['http://sns-webpic-qc.xhscdn.com/202504302109/277cd055ade888fd5503995b969c6f13/1040g00831bj07f3n0s004a7b4hg6io5ltor4dl0!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202504302109/caf140a83a0ef7bd6f850079980cdbc2/1040g00831bj07f3n0s0g4a7b4hg6io5lqiapifg!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202504302109/0cb183fdaa45f0b8a901562ee6514441/1040g00831bj07f3n0s104a7b4hg6io5llgjq2e8!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202504302109/3dd4f27f997f966a6ac9ae90801f8989/1040g00831bj07f3n0s1g4a7b4hg6io5lihj2j90!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202504302109/bb02c87faf3dbf5e4aec7af90af17b55/1040g00831bj07f3n0s204a7b4hg6io5lu9ifjvo!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202504302109/73d52da348db04408c872354d1b59ffe/1040g00831bj07f3n0s2g4a7b4hg6io5l9s9fv60!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202504302109/21c16674cb4f2e5692f70706d36947cb/1040g00831bj07f3n0s304a7b4hg6io5lklkc8c0!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202504302109/80b1ce91558a65c6b282db94a1cfe576/1040g00831bj07f3n0s3g4a7b4hg6io5l1d5bcso!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202504302109/ad0a6346aecd70a5742f81c60c29a1d5/1040g00831bj07f3n0s404a7b4hg6io5ljcl84r8!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202504302109/3d586bb25b6c55cee714e4975ac3defd/1040g00831bj07f3n0s4g4a7b4hg6io5l2nqsr7g!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202504302109/904f848737e48824d7ccea0eef8cb57d/1040g00831bj07f3n0s504a7b4hg6io5l56sdid8!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202504302109/ac4b27b1ef21d8bb88807abea759d4a6/1040g00831bj07f3n0s5g4a7b4hg6io5lntmcm8g!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202504302109/f1def8667f21a2dfac4bd03f40c690e5/1040g00831bj07f3n0s604a7b4hg6io5lvhuad9o!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202504302109/0667ffc16e6f8684f38294ec7432e86c/1040g00831bj07f3n0s6g4a7b4hg6io5llgtbf7o!nd_dft_wlteh_webp_3']</t>
+          <t>['http://sns-webpic-qc.xhscdn.com/202505012057/4dd98367af7eef26b8656d93951b83e8/1040g00831bj07f3n0s004a7b4hg6io5ltor4dl0!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202505012057/9be41aa5f409e9f392982ec6d3c176c2/1040g00831bj07f3n0s0g4a7b4hg6io5lqiapifg!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202505012057/e26bea8e7151c88cfe96034bbd4c024a/1040g00831bj07f3n0s104a7b4hg6io5llgjq2e8!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202505012057/87b1869a9e85c73c1ed40cd84688d0c4/1040g00831bj07f3n0s1g4a7b4hg6io5lihj2j90!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202505012057/3fcb69bc38a9b37c23d6f258275ab562/1040g00831bj07f3n0s204a7b4hg6io5lu9ifjvo!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202505012057/ff8755936501ae442d2b7a80c7132626/1040g00831bj07f3n0s2g4a7b4hg6io5l9s9fv60!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202505012057/19b8c622cab7a3048ed8bfd9b6c9f35b/1040g00831bj07f3n0s304a7b4hg6io5lklkc8c0!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202505012057/1fd629bad4af9d7e53e0f80b93ef6993/1040g00831bj07f3n0s3g4a7b4hg6io5l1d5bcso!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202505012057/7ed90da98aca1d58490e19580cd4556b/1040g00831bj07f3n0s404a7b4hg6io5ljcl84r8!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202505012057/24e2de195a013db18470baa0cc095b19/1040g00831bj07f3n0s4g4a7b4hg6io5l2nqsr7g!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202505012057/fad99ed7bb6b116dee1261c2d3ee5f2d/1040g00831bj07f3n0s504a7b4hg6io5l56sdid8!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202505012057/2ded8f075fb3a787a6a9324e69bec426/1040g00831bj07f3n0s5g4a7b4hg6io5lntmcm8g!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202505012057/9d03e34d44a8fcb81c3982142af6ba4b/1040g00831bj07f3n0s604a7b4hg6io5lvhuad9o!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202505012057/4bb08f2ee05a466ad0a26a308c7f007b/1040g00831bj07f3n0s6g4a7b4hg6io5llgtbf7o!nd_dft_wlteh_webp_3']</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
@@ -723,99 +723,92 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>6731b8fb000000001b02a2e0</t>
+          <t>671dfebb000000001402cf52</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://www.xiaohongshu.com/explore/6731b8fb000000001b02a2e0?xsec_token=ABL1SQy2MXgqhnSb1mTKXdEXxNTgRqNZ2vWWKickbxYZQ=</t>
+          <t>https://www.xiaohongshu.com/explore/671dfebb000000001402cf52?xsec_token=ABq4WDrhlzGas7P34ha1Kt6YM75wiVLly3Z74eLvteec0=</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>图集</t>
+          <t>视频</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>61178efe000000000101d3c0</t>
+          <t>61dad8d2000000001000fc2a</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>https://www.xiaohongshu.com/user/profile/61178efe000000000101d3c0</t>
+          <t>https://www.xiaohongshu.com/user/profile/61dad8d2000000001000fc2a</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>容小文</t>
+          <t>西边瓷小姐</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>https://sns-avatar-qc.xhscdn.com/avatar/1040g2jo31ehcs21u0c005o8nhrv0bku0qajbbi0</t>
+          <t>https://sns-avatar-qc.xhscdn.com/avatar/1040g2jo313o9n0hl1e005oeqr3941v1anuuamq0</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>2024瓷器挑选全攻略，为了身体，只选安心的</t>
+          <t>误入仙境的杯杯，太美了！💓（源头厂家）</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>瓷器怎么选呢？
-自从我做了攻略，我家那些花花绿绿的，明显能摸到纹路的瓷器就睡垃圾桶去了。
-现在吃饭的换成了纯白的，盘子换了釉中彩的和釉下彩的。
-觉得安心了不少。
-虽然有人说，能上市的都是合标的，但是连配料表都能...
-所以还是自己学点知识比较好。
-姐妹们，你们用的哪种呢？
-#瓷器[话题]#  #陶瓷碗[话题]#  #陶瓷盘子[话题]#  #骨瓷[话题]#  #碗[话题]#  #餐具[话题]#  #涨知识[话题]#  #不懂就问有问必答[话题]#</t>
+          <t>#手绘陶瓷[话题]# #手工艺[话题]# #瓷器[话题]# #老物件老情怀[话题]# #爱来自瓷器[话题]# #高端陶瓷[话题]# #陶瓷餐具[话题]# #陶瓷艺术[话题]# #源头工厂[话题]# #陶瓷马克杯[话题]#</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>360</t>
+          <t>3762</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>377</t>
+          <t>1357</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>36</t>
+          <t>107</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>74</t>
+          <t>531</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>http://sns-webpic-qc.xhscdn.com/202505012057/e9786c361f3eba1b0b645d0eace0393a/1040g2sg319evin0ame705oeqr3941v1a52tiv08!nd_dft_wlteh_webp_3</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>https://sns-video-bd.xhscdn.com/1040g2so319evin0fmg705oeqr3941v1ap1i3obo</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>['http://sns-webpic-qc.xhscdn.com/202504302109/79a768c61484837e7ab967b10520380e/spectrum/1040g0k031a27rgpq6u005o8nhrv0bku0n1r2f3o!nd_dft_wlteh_webp_3']</t>
+          <t>['http://sns-webpic-qc.xhscdn.com/202505012057/e9786c361f3eba1b0b645d0eace0393a/1040g2sg319evin0ame705oeqr3941v1a52tiv08!nd_dft_wlteh_webp_3']</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>['瓷器', '陶瓷碗', '陶瓷盘子', '骨瓷', '碗', '餐具', '涨知识', '不懂就问有问必答']</t>
+          <t>['手绘陶瓷', '手工艺', '瓷器', '老物件老情怀', '爱来自瓷器', '高端陶瓷', '陶瓷餐具', '陶瓷艺术', '源头工厂', '陶瓷马克杯']</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>2024-11-11 15:57:47</t>
+          <t>2024-10-27 16:50:03</t>
         </is>
       </c>
       <c r="S4" t="inlineStr">
@@ -832,7 +825,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>https://www.xiaohongshu.com/explore/67529c2b000000000203a427?xsec_token=ABc4yiUYUyUeyrKajZ0X1WeI5WFFzyyv37GM8CQ3ghm6Q=</t>
+          <t>https://www.xiaohongshu.com/explore/67529c2b000000000203a427?xsec_token=ABc4yiUYUyUeyrKajZ0X1WeHQuMnrKTbqs9g4eghhhgfY=</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -872,12 +865,12 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>494</t>
+          <t>501</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>208</t>
+          <t>210</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
@@ -902,7 +895,7 @@
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>['http://sns-webpic-qc.xhscdn.com/202504302109/a72884c7ff17ce998c7ec90bffa2d3f2/1040g00831b2bppgana005od9etc41eqqkgljlf8!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202504302109/f4c13bbf1de16387f9f04658627c52e1/1040g00831b2bppgana0g5od9etc41eqqu68ok8g!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202504302109/77a25c23aaa6947a749d433e55480e20/1040g00831b2bppgana105od9etc41eqq436imjg!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202504302109/314f7f917be863a6ef0632d9aafa1217/1040g00831b2bppgana1g5od9etc41eqqt9kb510!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202504302109/bdd31ccfb82c33472795c37ee287171c/1040g00831b2bppgana205od9etc41eqqjemr5k0!nd_dft_wlteh_webp_3']</t>
+          <t>['http://sns-webpic-qc.xhscdn.com/202505012057/bbebcac02edbd49d2714732d8087e080/1040g00831b2bppgana005od9etc41eqqkgljlf8!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202505012057/16d42ca357286c593c733991e8c68d10/1040g00831b2bppgana0g5od9etc41eqqu68ok8g!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202505012057/24dc38445de0ef0b4b4c07cc19b84f00/1040g00831b2bppgana105od9etc41eqq436imjg!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202505012057/85d59a29b0b18dfb496f9332e2dab8c4/1040g00831b2bppgana1g5od9etc41eqqt9kb510!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202505012057/5cdb50ed0151ea83d1b44ef761f05c36/1040g00831b2bppgana205od9etc41eqqjemr5k0!nd_dft_wlteh_webp_3']</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
@@ -924,12 +917,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>680d00ec000000001d01fdc1</t>
+          <t>674f00240000000007029a0e</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>https://www.xiaohongshu.com/explore/680d00ec000000001d01fdc1?xsec_token=ABzaoK5UZBUSFyoUPayX8VjOk6lQf0UZ48ukCmu5oDVJw=</t>
+          <t>https://www.xiaohongshu.com/explore/674f00240000000007029a0e?xsec_token=ABmbJ4OA8ywL_mwTr6zja0Gu9PMbHCXA2cCYXQPanimUE=</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -939,54 +932,55 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>6184a305000000001000cfa9</t>
+          <t>56a1b97a4775a70d06eefacc</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>https://www.xiaohongshu.com/user/profile/6184a305000000001000cfa9</t>
+          <t>https://www.xiaohongshu.com/user/profile/56a1b97a4775a70d06eefacc</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>静水</t>
+          <t>秋水集雅轩</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>https://sns-avatar-qc.xhscdn.com/avatar/1040g2jo30vbeh7khli605oc4kc2k1jt948ui2ng</t>
+          <t>https://sns-avatar-qc.xhscdn.com/avatar/1040g2jo319imcvsen200458tklsnlumc7ffeoc8</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>先进陶瓷材料行业分析（四）</t>
+          <t>一图看懂明清瓷器多种器型</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>烧结是陶瓷材料真正成为材料的一个关键步骤 ，烧结使原来的多孔坯体经致密化、晶粒成长、界面形成等过程得以发展形成显微结构，得到具有较高密度和强度的材料，而先进陶瓷属于脆性材料，缺乏金属材料的塑性 ，因此也需要独特的加工工艺。
-下期我们将进行先进陶瓷的产业链分析，欢迎大家关注[萌萌哒R]
-﻿#新材料[话题]#﻿ ﻿#先进陶瓷[话题]#﻿</t>
+          <t>[红色心形R]明,清两代的瓷器生产,在全国是以景德镇为中心区域,是中华民族瓷器创作的繁荣时期,也是我国陶瓷发展史上的高峰阶段。[火R]
+明清两代瓷器烧制在继承唐宋元传统工艺美术的背景和当时人们丰富创造力的基础上在瓷器的造型创新上有着巨大的成就。明清两代552年的历史长河中设计制作出许多优秀的造型样式,积累了丰富多样的处理手法，留存下来的大量的实物资料一直保存到今天,为我们的研究和学习提供了方便。
+我整理的几张图片是明清官窑和民窑比较经典和常见的器型，与大家分享[doge]
+﻿#老瓷器收藏[话题]#﻿ ﻿#古董瓷器[话题]#﻿ ﻿#瓷器收藏[话题]#﻿ ﻿#明清瓷器[话题]#﻿ ﻿#青花瓷[话题]#﻿ ﻿#兴趣榜样[话题]#﻿</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1258</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1437</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>43</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>198</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
@@ -1001,437 +995,20 @@
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>['http://sns-webpic-qc.xhscdn.com/202504302109/cbc406f7b93e0a0441d72170d1b3f0c5/spectrum/1040g0k031gocgsqd3c005oc4kc2k1jt9bar7png!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202504302109/b8bd8f23b9dab56d58d1f404623d7240/spectrum/1040g0k031gocgsqd3c0g5oc4kc2k1jt9m5fgoeo!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202504302109/9eef837200aef0120386a973a349bb2b/spectrum/1040g0k031gocgsqd3c105oc4kc2k1jt9ik2rfa0!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202504302109/b291cc3e905897caeea4f727f863556b/spectrum/1040g0k031gocgsqd3c1g5oc4kc2k1jt98bc2c30!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202504302109/1a342bac7483277fffb6dc510b8a8934/spectrum/1040g0k031gocgsqd3c205oc4kc2k1jt95u6s6lo!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202504302109/73706b9239c155f5d56f338b1eb0fa36/spectrum/1040g0k031gocgsqd3c2g5oc4kc2k1jt9phdil0o!nd_dft_wlteh_webp_3']</t>
+          <t>['http://sns-webpic-qc.xhscdn.com/202505012057/27c33c4af262c4afe6f03c07430c3b9d/spectrum/1040g0k031auqh9qk6q00458tklsnlumce7o4i2o!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202505012057/05f857d5cb24ed5804d97c6463fc1edb/spectrum/1040g0k031auqh5f96u10458tklsnlumc4llmsgo!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202505012057/61bf2f1922c3ba7e025f56313c5246dc/spectrum/1040g0k031auqh5f96u0g458tklsnlumc6ebj9j8!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202505012057/945e7a5e5e141f1eccd8c1f801b54560/spectrum/1040g0k031auqh5f96u00458tklsnlumc35tua8g!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202505012057/e5c5c57f1548de85e2ec7179bd16c871/spectrum/1040g0k031auqh9qk6q0g458tklsnlumc3it3r80!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202505012057/5c1723bb07f0c25b3d6f2cd5a7d8dd7d/spectrum/1040g0k031auqh9qk6q1g458tklsnlumcsq3dva8!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202505012057/caeb1d3a8fc11f8d41c518e24a5de388/1040g2sg31aura08pnee0458tklsnlumcp06k24g!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202505012057/e1d8fb8f186c5323662f0376cf151dc8/spectrum/1040g0k031auqh9qk6q10458tklsnlumcjj2nuh0!nd_dft_wlteh_webp_3']</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>['新材料', '先进陶瓷']</t>
+          <t>['老瓷器收藏', '古董瓷器', '瓷器收藏', '明清瓷器', '青花瓷', '兴趣榜样']</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
         <is>
-          <t>2025-04-30 20:01:32</t>
+          <t>2024-12-03 20:57:08</t>
         </is>
       </c>
       <c r="S6" t="inlineStr">
-        <is>
-          <t>湖南</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>67b15757000000002902bcce</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>https://www.xiaohongshu.com/explore/67b15757000000002902bcce?xsec_token=ABISfWP1t4qOEeMEw4j5JVPLAeQS49LQDMNYQ5DZ2Ib64=</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>图集</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>60ebab9d0000000001007461</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>https://www.xiaohongshu.com/user/profile/60ebab9d0000000001007461</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>小茉莉🍪</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>https://sns-avatar-qc.xhscdn.com/avatar/1040g2jo31du2843i10105o7bleeg8t317jk1v7o</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>✨DIY成功了……‼️ |太好看成就感爆棚🎉</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>好喜欢今天和朋友一起去diy的这个碗[哇R]太好看了[偷笑R]
-其实也没想象的那么难[害羞R]
-想看看你们喜欢的碗长啥样🤔[暗中观察R]
-💡总结：这次DIY体验真的太棒了，它让我挖掘出了自己动手能力的一面。以后我打算尝试更多不同类型的DIY，继续享受这种创造的乐趣。也想鼓励大家都去试试DIY，说不定会发现一个不一样的自己[大笑R][大笑R][大笑R]
-#这个碗好看[PK]# @薯条小助手
-#餐具[话题]# #手工diy[话题]##好看的碗[话题]# #每日分享[话题]# #好看的餐具[话题]# #生活好物[话题]# #感想[话题]##记录吧就现在[话题]# #生活需要分享[话题]#</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>4406</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>2107</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>203</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>924</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="P7" t="inlineStr">
-        <is>
-          <t>['http://sns-webpic-qc.xhscdn.com/202504302109/bd6ea4aa03214be90b984132f6c6902a/1040g2sg31dus8q9cgk705o7bleeg8t313lmph4o!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202504302109/a54df42f956250c8341b839dd84e182d/notes_pre_post/1040g3k831durpg81gs905o7bleeg8t31rfcs4oo!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202504302109/5ffa942a5dba8ca749ba9eb0fe0f0cdd/notes_pre_post/1040g3k831durpg81gs9g5o7bleeg8t31hhk0r5g!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202504302109/418376ed748a41534e66a61d6db13c83/notes_pre_post/1040g3k831durpg81gsa05o7bleeg8t31uuaoopo!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202504302109/8d4512531a8b1bfbb1ed9a50f22747d2/notes_pre_post/1040g3k831durpg81gsag5o7bleeg8t31560o3q0!nd_dft_wlteh_webp_3']</t>
-        </is>
-      </c>
-      <c r="Q7" t="inlineStr">
-        <is>
-          <t>['餐具', '手工diy', '好看的碗', '每日分享', '好看的餐具', '生活好物', '感想', '记录吧就现在', '生活需要分享']</t>
-        </is>
-      </c>
-      <c r="R7" t="inlineStr">
-        <is>
-          <t>2025-02-16 11:11:19</t>
-        </is>
-      </c>
-      <c r="S7" t="inlineStr">
-        <is>
-          <t>未知</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>663aef08000000001e033a48</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>https://www.xiaohongshu.com/explore/663aef08000000001e033a48?xsec_token=ABXRVhiDEdrz7A-WjKfklpkYNcvYLh0qoPkeE722KIGEk=</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>图集</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>5d2586a1000000001202554d</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>https://www.xiaohongshu.com/user/profile/5d2586a1000000001202554d</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>桃汁拌茅台</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>https://sns-avatar-qc.xhscdn.com/avatar/1040g2jo31468knkb26005n95gqgkkladpo77jng</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>男朋友：你敢砍我都不敢听🥹（右划附价格❗️）</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>每次一开始砍价npy就跑出店等我拎着战利品出来🥹真的进了景德镇就别想空着手出来！
-🙋我一共逛了三个市集，来总结一下～
-1️⃣陶溪川
-因为我是5.6去的，市集都结束了，只有街边的小店开着，基本都是比较艺术的被子茶具，往里逛也有可爱的摆件，价格普遍不便宜，孤品偏多。
-2️⃣雕塑瓷厂
-这是我觉得最好逛的😍街边基本都是批发的瓶瓶罐罐，价格中等，一些巷子拐进去会有艺术家个人设计的小店，真的都特别可爱😍（p3的上面两个）但是价格稍微偏贵一些，可以大胆讨价还价！店主人都蛮好的嘿嘿😋然后这里有很多拍照打卡点，建议穿彩色！（p5-10）
-3️⃣陶阳新村
-这是一个纯批发的市集，很少有个人设计，价格也是最便宜的！我就住在这附近的民宿，所以第一天先草草看了一遍有什么品，第二天去其他两个地方看到一样的品就不会被宰！这里价格都比较统一所以很难还价。
-快来交换一张你们的战利品👀
-#旅游[话题]# #景德镇陶瓷[话题]# #景德镇市集攻略[话题]# #旅游攻略[话题]##陶阳新村[话题]# #雕塑瓷厂探店[话题]# #陶溪川[话题]# #好物推荐[话题]# #家居饰品[话题]# #装饰品[话题]# #购物[话题]# #杯子收藏[话题]# #陶瓷艺术[话题]# #交换一张你在景德镇淘到的瓷器[话题]# #交换一张景德镇的照片[话题]# #景德镇攻略[话题]#</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>1506</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>767</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>195</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>717</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="P8" t="inlineStr">
-        <is>
-          <t>['http://sns-webpic-qc.xhscdn.com/202504302109/136e2db254ae6b0c17a86704d83bab81/1040g2sg312h7tdv41i005n95gqgkkladu2hq4k0!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202504302109/89c94dc0a8636cb186af94f6755d7360/1040g2sg312h7tdv41i0g5n95gqgkkladt9h81b8!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202504302109/d547ee2e88d08fc7ee5414c02d0eb351/1040g2sg312h7tdv41i105n95gqgkkladku3p5cg!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202504302109/2a4df9a4d9c4add624f5cb0b1463bc17/1040g2sg312h7tdv41i1g5n95gqgkklad1ukgumg!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202504302109/8215d286731222c97d3e6bfabf99d947/1040g2sg312h7tdv41i205n95gqgkklad2hovrm0!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202504302109/d6f38d6898a4f5d83bf1401371fe0c18/1040g2sg312h7tdv41i2g5n95gqgkkladqog2a40!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202504302109/c2648f799893052213bec74c303fff1a/1040g2sg312h7tdv41i305n95gqgkklad8ccdmf8!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202504302109/64c3527d8222bfae60f0b9a23e0b601a/1040g2sg312h7tdv41i3g5n95gqgkkladrntafa8!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202504302109/34f1d3f5e9b1d8f0fe3992723712820d/1040g2sg312h7tdv41i405n95gqgkkladivhttd8!nd_dft_wgth_webp_3', 'http://sns-webpic-qc.xhscdn.com/202504302109/841cb8ed2871b2d9fb672f16d3d92d89/1040g2sg312h7tdv41i4g5n95gqgkkladjl3pr5g!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202504302109/4221df4ae0895f33e86324c514ed8e75/1040g2sg312h7tdv41i505n95gqgkkladfbpmp80!nd_dft_wgth_webp_3', 'http://sns-webpic-qc.xhscdn.com/202504302109/05615598f52b5c2041050ac1373d99d8/1040g2sg312h7tdv41i5g5n95gqgkkladuejv31g!nd_dft_wlteh_webp_3']</t>
-        </is>
-      </c>
-      <c r="Q8" t="inlineStr">
-        <is>
-          <t>['旅游', '景德镇陶瓷', '景德镇市集攻略', '旅游攻略', '陶阳新村', '雕塑瓷厂探店', '陶溪川', '好物推荐', '家居饰品', '装饰品', '购物', '杯子收藏', '陶瓷艺术', '交换一张你在景德镇淘到的瓷器', '交换一张景德镇的照片', '景德镇攻略']</t>
-        </is>
-      </c>
-      <c r="R8" t="inlineStr">
-        <is>
-          <t>2024-05-08 12:16:02</t>
-        </is>
-      </c>
-      <c r="S8" t="inlineStr">
-        <is>
-          <t>未知</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>64aa3757000000002f0274c8</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>https://www.xiaohongshu.com/explore/64aa3757000000002f0274c8?xsec_token=ABgA6EkP0UWFen8upPh5z3IYxK_yhJ0R4UwD6nrBOlWfY=</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>图集</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>649e4ff0000000001001c8aa</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>https://www.xiaohongshu.com/user/profile/649e4ff0000000001001c8aa</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>福州🥇惠万家瓷砖总店</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>https://sns-avatar-qc.xhscdn.com/avatar/1040g2jo30sdg3qar3c005p4u9vo43i5a3v62h38</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>感谢阿姐发来的反馈图👍🏻【福州惠万家陶瓷】</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>感谢阿姐对惠万家陶瓷的高度评价，好砖质量看的见，釉面也好[郁金香R][哇R][哇R]
-#福州瓷砖[话题]# #福州瓷砖仓库[话题]# #福州网红瓷砖店[话题]# #福州性价比瓷砖[话题]# #福州瓷砖店[话题]# #福州惠万家陶瓷[话题]# #福州瓷砖惠万家陶瓷[话题]# #福州宝藏瓷砖店[话题]# #福州惠万家陶瓷厂家直销[话题]# #福州装修推荐[话题]# #福州装修施工[话题]# #福州自装[话题]# #福州自装日记[话题]##福州[话题]# #福州瓷砖店[话题]# #福州瓷砖选择[话题]# #福州装修设计施工[话题]##福州装修[话题]# #福州装修施工[话题]##福州装修[话题]#</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="P9" t="inlineStr">
-        <is>
-          <t>['http://sns-webpic-qc.xhscdn.com/202504302109/128a920efda6d5f9b66cf02f177e28fe/1000g0082p7ltt8ujq0dg5p4u9vo43i5atd63evg!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202504302109/e775aba7773c384d8c16f8105583921a/1000g0082p7m000qjq0005p4u9vo43i5asa7ku70!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202504302109/e3323958b3e114b0bd03c99f6af191a8/1000g0082p7m000qjq00g5p4u9vo43i5a8nna9c0!nd_dft_wgth_webp_3', 'http://sns-webpic-qc.xhscdn.com/202504302109/bded31ceb3f229a2b64c5f998e49a144/1000g0082p7m000qjq0105p4u9vo43i5aagpme20!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202504302109/a16168e77aa97579383e2fe85fc75e64/1000g0082p7m000qjq01g5p4u9vo43i5a29kbt98!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202504302109/c0a06d6b00533dc3a559b33407110455/1000g0082p7m000qjq0205p4u9vo43i5ambe32to!nd_dft_wgth_webp_3']</t>
-        </is>
-      </c>
-      <c r="Q9" t="inlineStr">
-        <is>
-          <t>['福州瓷砖', '福州瓷砖仓库', '福州网红瓷砖店', '福州性价比瓷砖', '福州瓷砖店', '福州惠万家陶瓷', '福州瓷砖惠万家陶瓷', '福州宝藏瓷砖店', '福州惠万家陶瓷厂家直销', '福州装修推荐', '福州装修施工', '福州自装', '福州自装日记', '福州', '福州瓷砖选择', '福州装修设计施工', '福州装修']</t>
-        </is>
-      </c>
-      <c r="R9" t="inlineStr">
-        <is>
-          <t>2023-07-09 12:28:07</t>
-        </is>
-      </c>
-      <c r="S9" t="inlineStr">
-        <is>
-          <t>未知</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>67bb3d69000000002503e200</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>https://www.xiaohongshu.com/explore/67bb3d69000000002503e200?xsec_token=ABZPnZq6VvAWkn8e0xHcYUdYEg0bfejAwVPCGr0C6YNlw=</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>图集</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>651977bf000000002402d91a</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>https://www.xiaohongshu.com/user/profile/651977bf000000002402d91a</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>流年苏</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>https://sns-avatar-qc.xhscdn.com/avatar/1040g2jo31e8e73kc0u6g5p8peuvp5m8qf04bl00</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>被这家店治愈了‼️🪑</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>#把时间浪费在美好的事物上[话题]#
-1.泥与火的交响
-在陶艺的世界里，每一次旋转都是泥土与火的对话，每一次塑形都是匠人情感的流露。从泥巴到成品，每一步都充满了无限可能。
-2. 创意与传统的融合
-陶艺不仅是对传统的传承，更是对创意的探索。在这里，你可以将古老的技艺与现代的设计思维相结合，创造出独一无二的艺术品。
-3. 静心与修身的过程
-陶艺制作需要耐心和细致，它是一种静心的修炼，也是一种精神的升华。在这个过程中，你会发现自己的内心更加平和，生活更加充实。
-4.艺术与生活的桥梁
-陶艺不仅仅是艺术的表现，更是生活的一部分。无论是日常使用的餐具，还是装饰家居的艺术品，陶艺都能为你的生活增添一份独特的情调。
-陶艺，是一种文化的传承，一种生活的态度，一种个性的展现。让我们一起，用双手塑造生活的美好。
-[看R]周末休闲好去处，约上三五好友一期玩泥巴
-📍地址：福清宏路有元艺术工作室——元器｜陶社
-🅿️门口有车位可以停车
-🕒本周末特别延长至23:00
-[红色心形R][红色心形R]记得提前预约哦#福清[话题]# #福清探店[话题]# #元器陶社[话题]# #有元艺术工作室[话题]# #陶艺[话题]# #福清拍照圣地[话题]# #陶艺家手作[话题]# #手作陶瓷[话题]# #陶艺diy[话题]#</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="P10" t="inlineStr">
-        <is>
-          <t>['http://sns-webpic-qc.xhscdn.com/202504302109/d7a9df82039bb1a71a5be23163ffe4bd/1040g00831e8e6tb40u6g5p8peuvp5m8qa0lc1t0!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202504302109/6385d4a0978072a207678301f1b2f09e/1040g2sg31e8e6targudg5p8peuvp5m8q7juqm10!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202504302109/35b2d8d0e5fe2e585beed1ad473a9b93/1040g2sg31e8e6tco0sd05p8peuvp5m8qvaqdbng!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202504302109/9e843a6aa7bc53459928725d62ffae32/1040g2sg31e8e6tb0gsdg5p8peuvp5m8qa42fbj8!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202504302109/f33d50abefbbe29a66c73e0ac1c21b7e/1040g00831e8e6tau0k6g5p8peuvp5m8qip7h7ag!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202504302109/dc142204c6671898a261a97da521a547/1040g00831e8e6tc90u6g5p8peuvp5m8q7ul310g!nd_dft_wlteh_webp_3', 'http://sns-webpic-qc.xhscdn.com/202504302109/0309488044d43b52c9a4cd9ea8bac6ba/1040g2sg31e8e6tauh0d05p8peuvp5m8q0clamt8!nd_dft_wlteh_webp_3']</t>
-        </is>
-      </c>
-      <c r="Q10" t="inlineStr">
-        <is>
-          <t>['把时间浪费在美好的事物上', '福清', '福清探店', '元器陶社', '有元艺术工作室', '陶艺', '福清拍照圣地', '陶艺家手作', '手作陶瓷', '陶艺diy']</t>
-        </is>
-      </c>
-      <c r="R10" t="inlineStr">
-        <is>
-          <t>2025-02-23 23:23:21</t>
-        </is>
-      </c>
-      <c r="S10" t="inlineStr">
         <is>
           <t>未知</t>
         </is>

</xml_diff>